<commit_message>
Fix vaccination template by removing address information from first sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/csv/template_vaccination.xlsx
+++ b/src/test/resources/csv/template_vaccination.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cedricmoullet/sandbox/CovidCertificate-Management-Service/src/test/resources/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CE51A0-64DA-7144-AF1F-F3F5A8626BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C83BCEE-2A05-6649-AC17-D2AF9C154FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>givenName</t>
   </si>
@@ -928,7 +928,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -938,18 +938,14 @@
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -963,34 +959,22 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1004,30 +988,18 @@
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F2">
-        <v>1234</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1">
+        <v>44344</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-      <c r="L2" s="1">
-        <v>44344</v>
-      </c>
-      <c r="M2" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>